<commit_message>
staff hours are now fortnightly
</commit_message>
<xml_diff>
--- a/data/shifty.xlsx
+++ b/data/shifty.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -58,43 +58,70 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Hew Level</t>
+    <t xml:space="preserve">Hew</t>
   </si>
   <si>
     <t xml:space="preserve">AAL?</t>
   </si>
   <si>
-    <t xml:space="preserve">Average Weekly Hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mon start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mon end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tue start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tue end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wed start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wed end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thu start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thu end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fri start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fri end</t>
+    <t xml:space="preserve">Mon 1 start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon 1 end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue 1 start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue 1 end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed 1 start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed 1 end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu 1 start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu 1 end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri 1 start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri 1 end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon 2 start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon 2 end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue 2 start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue 2 end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed 2 start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed 2 End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu 2 start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu 2 end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri 2 start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri 2 end</t>
   </si>
   <si>
     <t xml:space="preserve">y</t>
@@ -283,10 +310,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8622448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="14.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="18.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.3469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="14.8928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -393,17 +420,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="14.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.57142857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.05612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.5"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.8979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.1683673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.3826530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.1428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.4132653061225"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.93367346938776"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.32142857142857"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.5"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="10.8979591836735"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10.1683673469388"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="11.3826530612245"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.8979591836735"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="11.1428571428571"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="10.4132653061225"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="9.93367346938776"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="9.32142857142857"/>
+    <col collapsed="false" hidden="false" max="1023" min="24" style="1" width="14.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="14.8928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -416,7 +463,7 @@
       <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="8" t="s">
@@ -449,10 +496,33 @@
       <c r="N1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
+      <c r="O1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
@@ -462,75 +532,107 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="6" t="n">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0.333333333333333</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>0.333333333333333</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="F2" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="G2" s="5" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="G2" s="5" t="n">
-        <v>0.333333333333333</v>
-      </c>
       <c r="H2" s="5" t="n">
+        <v>0.354166666666667</v>
+      </c>
+      <c r="I2" s="5" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="I2" s="5" t="n">
+      <c r="J2" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="N2" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="O2" s="5" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="P2" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="Q2" s="5" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="R2" s="5" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="J2" s="5" t="n">
+      <c r="S2" s="5" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="K2" s="5" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="L2" s="5" t="n">
+      <c r="T2" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="U2" s="5" t="n">
         <v>0.6875</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
+      <c r="V2" s="5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="W2" s="5" t="n">
+        <v>0.6875</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>20</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
+      <c r="J3" s="5" t="n">
+        <v>0.479166666666667</v>
+      </c>
       <c r="K3" s="5" t="n">
-        <v>0.479166666666667</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="L3" s="5" t="n">
-        <v>0.833333333333333</v>
+        <v>0.354166666666667</v>
       </c>
       <c r="M3" s="5" t="n">
-        <v>0.354166666666667</v>
-      </c>
-      <c r="N3" s="5" t="n">
         <v>0.708333333333333</v>
       </c>
+      <c r="N3" s="9"/>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
+      <c r="R3" s="5" t="n">
+        <v>0.479166666666667</v>
+      </c>
+      <c r="S3" s="5" t="n">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="T3" s="5" t="n">
+        <v>0.354166666666667</v>
+      </c>
+      <c r="U3" s="5" t="n">
+        <v>0.708333333333333</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -556,9 +658,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="10" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="14.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="10" width="14.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="14.8928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -569,10 +671,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,9 +715,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="17.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="11.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.7551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="17.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="11.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
changing RDOs to leave, allowing leave to be specified in a range
</commit_message>
<xml_diff>
--- a/data/shifty.xlsx
+++ b/data/shifty.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Shifts" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Staff" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Negs" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="RDOs" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Leave" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -137,18 +137,22 @@
   </si>
   <si>
     <t xml:space="preserve">End time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Day</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY\ HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="167" formatCode="HH:MM:SS"/>
-    <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -236,20 +240,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -257,31 +277,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -305,104 +305,105 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="18.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.3469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.8367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="14.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="14.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+      <c r="A2" s="7" t="n">
         <v>42772</v>
       </c>
-      <c r="B2" s="5" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="C2" s="5" t="n">
+      <c r="B2" s="8" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="C2" s="8" t="n">
         <v>0.375</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="8" t="n">
         <v>0.375</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="8" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="8" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="7" t="n">
         <v>42773</v>
       </c>
-      <c r="B5" s="5" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="C5" s="5" t="n">
+      <c r="B5" s="8" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="C5" s="8" t="n">
         <v>0.375</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="8" t="n">
         <v>0.375</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="8" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -422,215 +423,215 @@
   </sheetPr>
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.57142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.05612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.5"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.1683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.3826530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.1428571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.93367346938776"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.32142857142857"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.5"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="10.8979591836735"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10.1683673469388"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="11.3826530612245"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.8979591836735"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="11.1428571428571"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="9.93367346938776"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="9.32142857142857"/>
-    <col collapsed="false" hidden="false" max="1023" min="24" style="1" width="14.8928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="14.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="2" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="2" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1023" min="24" style="3" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="14.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="5" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E2" s="5" t="n">
+      <c r="D2" s="8" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E2" s="8" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="F2" s="5" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="G2" s="5" t="n">
+      <c r="F2" s="8" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="G2" s="8" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="H2" s="8" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="I2" s="5" t="n">
+      <c r="I2" s="8" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="J2" s="5" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="K2" s="5" t="n">
+      <c r="J2" s="8" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="K2" s="8" t="n">
         <v>0.6875</v>
       </c>
-      <c r="N2" s="5" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="O2" s="5" t="n">
+      <c r="N2" s="8" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="O2" s="8" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="P2" s="5" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="Q2" s="5" t="n">
+      <c r="P2" s="8" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="Q2" s="8" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="R2" s="5" t="n">
+      <c r="R2" s="8" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="S2" s="5" t="n">
+      <c r="S2" s="8" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="T2" s="5" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="U2" s="5" t="n">
+      <c r="T2" s="8" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="U2" s="8" t="n">
         <v>0.6875</v>
       </c>
-      <c r="V2" s="5" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="W2" s="5" t="n">
+      <c r="V2" s="8" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="W2" s="8" t="n">
         <v>0.6875</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="5" t="n">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="8" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="K3" s="5" t="n">
+      <c r="K3" s="8" t="n">
         <v>0.833333333333333</v>
       </c>
-      <c r="L3" s="5" t="n">
+      <c r="L3" s="8" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="M3" s="5" t="n">
+      <c r="M3" s="8" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="5" t="n">
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="8" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="S3" s="5" t="n">
+      <c r="S3" s="8" t="n">
         <v>0.833333333333333</v>
       </c>
-      <c r="T3" s="5" t="n">
+      <c r="T3" s="8" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="U3" s="5" t="n">
+      <c r="U3" s="8" t="n">
         <v>0.708333333333333</v>
       </c>
     </row>
@@ -653,41 +654,41 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="10" width="14.8928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="14.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="14.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="7" t="n">
         <v>42773</v>
       </c>
-      <c r="C2" s="5" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="D2" s="5" t="n">
+      <c r="C2" s="8" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="D2" s="8" t="n">
         <v>0.375</v>
       </c>
     </row>
@@ -707,33 +708,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.7551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="17.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="11.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>0</v>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="7" t="n">
         <v>42773</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>42776</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>42781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new shift types - slc and reference
</commit_message>
<xml_diff>
--- a/data/shifty.xlsx
+++ b/data/shifty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Shifts" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -52,9 +52,15 @@
     <t xml:space="preserve">Backup</t>
   </si>
   <si>
+    <t xml:space="preserve">SLC</t>
+  </si>
+  <si>
     <t xml:space="preserve">ResponsibleOfficer</t>
   </si>
   <si>
+    <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
@@ -124,13 +130,28 @@
     <t xml:space="preserve">Fri 2 end</t>
   </si>
   <si>
+    <t xml:space="preserve">SLC?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard? (empty means yes)</t>
+  </si>
+  <si>
     <t xml:space="preserve">y</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rowena</t>
   </si>
   <si>
     <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
   </si>
   <si>
     <t xml:space="preserve">Start time</t>
@@ -154,7 +175,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -197,6 +218,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -240,7 +269,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -278,6 +307,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -302,19 +335,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="18.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="19.9897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="16.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="14.4183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,7 +421,7 @@
         <v>0.375</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E5" s="9"/>
     </row>
@@ -401,9 +434,20 @@
         <v>0.458333333333333</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="8" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -421,108 +465,120 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="2" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="2" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1023" min="24" style="3" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="14.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="5.20918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="5.69897959183674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.0255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="2" width="10.5408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.93367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="11.0255102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="10.4132653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="10.8979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="10.1683673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="9.81122448979592"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="9.08163265306122"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="11.0255102040816"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="2" width="10.5408163265306"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="9.93367346938776"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="11.0255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="10.5408163265306"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="10.8979591836735"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="10.1683673469388"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="9.81122448979592"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="9.08163265306122"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="3" width="6.36224489795918"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="3" width="11.9489795918367"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="27.5"/>
+    <col collapsed="false" hidden="false" max="1023" min="27" style="3" width="14.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="14.4183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,7 +589,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D2" s="8" t="n">
         <v>0.333333333333333</v>
@@ -589,23 +645,29 @@
       <c r="W2" s="8" t="n">
         <v>0.6875</v>
       </c>
+      <c r="X2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B3" s="9" t="n">
         <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+        <v>41</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
       <c r="J3" s="8" t="n">
         <v>0.479166666666667</v>
       </c>
@@ -618,10 +680,10 @@
       <c r="M3" s="8" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
       <c r="R3" s="8" t="n">
         <v>0.479166666666667</v>
       </c>
@@ -633,6 +695,12 @@
       </c>
       <c r="U3" s="8" t="n">
         <v>0.708333333333333</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -659,23 +727,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="14.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="14.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="14.4183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -710,27 +778,27 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="11.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="11.3826530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,7 +811,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>42776</v>

</xml_diff>

<commit_message>
payweek / nonpayweek is now displayed on each day of the roster
</commit_message>
<xml_diff>
--- a/data/shifty.xlsx
+++ b/data/shifty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Shifts" sheetId="1" state="visible" r:id="rId2"/>
@@ -76,64 +76,64 @@
     <t xml:space="preserve">AAL?</t>
   </si>
   <si>
-    <t xml:space="preserve">Mon 1 start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mon 1 end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tue 1 start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tue 1 end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wed 1 start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wed 1 end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thu 1 start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thu 1 end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fri 1 start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fri 1 end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mon 2 start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mon 2 end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tue 2 start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tue 2 end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wed 2 start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wed 2 End</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thu 2 start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thu 2 end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fri 2 start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fri 2 end</t>
+    <t xml:space="preserve">Mon start P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon end P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue start P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue end P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed start P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed end P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu start P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu end P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri start P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri end P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon start N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon end N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue start N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue end N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed start N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed End N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu start N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu end N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri start N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri end N</t>
   </si>
   <si>
     <t xml:space="preserve">SLC?</t>
@@ -343,8 +343,8 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -483,8 +483,8 @@
   </sheetPr>
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
now supports formulas on date fields
</commit_message>
<xml_diff>
--- a/data/shifty.xlsx
+++ b/data/shifty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Shifts" sheetId="1" state="visible" r:id="rId2"/>
@@ -587,8 +587,8 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -669,6 +669,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="n">
+        <f aca="false">A2+1</f>
         <v>42773</v>
       </c>
       <c r="B5" s="9" t="n">
@@ -727,36 +728,36 @@
   </sheetPr>
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="4.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="3" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="3" width="5.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="10.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="10.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="10.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="10.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="9.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="10.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="2" width="10.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="10.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="10.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="10.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="9.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="3" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="3" width="5.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="3" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="3" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="3" width="14.31"/>
@@ -1049,10 +1050,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="3" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="3" width="11.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
adding BEast shift type
</commit_message>
<xml_diff>
--- a/data/shifty.xlsx
+++ b/data/shifty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Shifts" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">Hew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beast</t>
   </si>
   <si>
     <t xml:space="preserve">Mon start P</t>
@@ -587,7 +590,7 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -726,10 +729,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -739,28 +742,29 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="3" width="5.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="9.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="2" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="9.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="3" width="5.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="3" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="3" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="3" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="2" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="2" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="3" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="3" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="3" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="3" width="14.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,7 +786,7 @@
       <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="7" t="s">
         <v>16</v>
       </c>
       <c r="H1" s="5" t="s">
@@ -842,9 +846,12 @@
       <c r="Z1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AA1" s="0"/>
+      <c r="AA1" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="AB1" s="0"/>
       <c r="AC1" s="0"/>
+      <c r="AD1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
@@ -854,120 +861,123 @@
         <v>5</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="9" t="n">
+        <v>37</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="9" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="H2" s="9" t="n">
+      <c r="I2" s="9" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="I2" s="9" t="n">
+      <c r="J2" s="9" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="J2" s="9" t="n">
+      <c r="K2" s="9" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="K2" s="9" t="n">
+      <c r="L2" s="9" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="L2" s="9" t="n">
+      <c r="M2" s="9" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="M2" s="9" t="n">
+      <c r="N2" s="9" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="N2" s="9" t="n">
+      <c r="O2" s="9" t="n">
         <v>0.6875</v>
       </c>
-      <c r="Q2" s="9" t="n">
+      <c r="R2" s="9" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="R2" s="9" t="n">
+      <c r="S2" s="9" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="S2" s="9" t="n">
+      <c r="T2" s="9" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="T2" s="9" t="n">
+      <c r="U2" s="9" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="U2" s="9" t="n">
+      <c r="V2" s="9" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="V2" s="9" t="n">
+      <c r="W2" s="9" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="W2" s="9" t="n">
+      <c r="X2" s="9" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="X2" s="9" t="n">
+      <c r="Y2" s="9" t="n">
         <v>0.6875</v>
       </c>
-      <c r="Y2" s="9" t="n">
+      <c r="Z2" s="9" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="Z2" s="9" t="n">
+      <c r="AA2" s="9" t="n">
         <v>0.6875</v>
       </c>
-      <c r="AA2" s="0"/>
       <c r="AB2" s="0"/>
       <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="10" t="n">
         <v>6</v>
       </c>
       <c r="C3" s="10"/>
       <c r="F3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="11"/>
+        <v>39</v>
+      </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="9" t="n">
+      <c r="M3" s="11"/>
+      <c r="N3" s="9" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="N3" s="9" t="n">
+      <c r="O3" s="9" t="n">
         <v>0.833333333333333</v>
       </c>
-      <c r="O3" s="9" t="n">
+      <c r="P3" s="9" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="P3" s="9" t="n">
+      <c r="Q3" s="9" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
-      <c r="U3" s="9" t="n">
+      <c r="U3" s="11"/>
+      <c r="V3" s="9" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="V3" s="9" t="n">
+      <c r="W3" s="9" t="n">
         <v>0.833333333333333</v>
       </c>
-      <c r="W3" s="9" t="n">
+      <c r="X3" s="9" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="X3" s="9" t="n">
+      <c r="Y3" s="9" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="AA3" s="0"/>
       <c r="AB3" s="0"/>
       <c r="AC3" s="0"/>
+      <c r="AD3" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1006,10 +1016,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,10 +1071,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1077,7 +1087,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="8" t="n">
         <v>42776</v>

</xml_diff>

<commit_message>
multiple shift types per shift
</commit_message>
<xml_diff>
--- a/data/shifty.xlsx
+++ b/data/shifty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Shifts" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard,Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -591,17 +597,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="C:C A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="18.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="19.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="25.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="3" width="14.31"/>
   </cols>
@@ -714,6 +720,20 @@
       </c>
       <c r="F7" s="3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -734,8 +754,8 @@
   </sheetPr>
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -773,13 +793,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>9</v>
@@ -794,67 +814,67 @@
         <v>6</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AC1" s="0"/>
       <c r="AD1" s="0"/>
@@ -871,16 +891,16 @@
         <v>0</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I2" s="9" t="n">
         <v>0.333333333333333</v>
@@ -942,7 +962,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="10" t="n">
         <v>6</v>
@@ -950,7 +970,7 @@
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="G3" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -1009,7 +1029,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C:C B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1021,16 +1041,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,7 +1086,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="C:C E18"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1079,13 +1099,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,7 +1118,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="8" t="n">
         <v>42776</v>

</xml_diff>

<commit_message>
Reason for negs & leave
</commit_message>
<xml_diff>
--- a/data/shifty.xlsx
+++ b/data/shifty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Shifts" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -160,10 +160,19 @@
     <t xml:space="preserve">End time</t>
   </si>
   <si>
+    <t xml:space="preserve">Reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not want to work</t>
+  </si>
+  <si>
     <t xml:space="preserve">First Day</t>
   </si>
   <si>
     <t xml:space="preserve">Last Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holiday</t>
   </si>
 </sst>
 </file>
@@ -175,7 +184,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -197,87 +206,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -308,57 +236,15 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -366,23 +252,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -406,189 +277,65 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -599,7 +346,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1026,17 +773,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="3" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="17.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="3" width="14.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,6 +800,9 @@
       <c r="D1" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="E1" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
@@ -1065,6 +816,9 @@
       </c>
       <c r="D2" s="9" t="n">
         <v>0.375</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1083,10 +837,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1102,10 +856,13 @@
         <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1115,6 +872,9 @@
       <c r="B2" s="8" t="n">
         <v>42773</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -1126,6 +886,7 @@
       <c r="C3" s="1" t="n">
         <v>42781</v>
       </c>
+      <c r="D3" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
can now exclude people from working a shift
</commit_message>
<xml_diff>
--- a/data/shifty.xlsx
+++ b/data/shifty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Shifts" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Manual Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excluded Names</t>
   </si>
   <si>
     <t xml:space="preserve">Label</t>
@@ -184,7 +187,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -226,6 +229,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -278,7 +289,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -311,19 +322,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -344,10 +359,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -356,7 +371,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="25.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="3" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="3" width="14.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,95 +394,106 @@
       <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="9" t="n">
         <v>42772</v>
       </c>
-      <c r="B2" s="9" t="n">
+      <c r="B2" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="10" t="n">
         <v>0.375</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="0"/>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9" t="n">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10" t="n">
         <v>0.375</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="10" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="0"/>
+      <c r="D3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="n">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="10" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="10"/>
+      <c r="D4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="9" t="n">
         <f aca="false">A2+1</f>
         <v>42773</v>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="10" t="n">
         <v>0.375</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="10"/>
+      <c r="D5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="n">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10" t="n">
         <v>0.375</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="10" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="10"/>
+      <c r="D6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="10" t="n">
         <v>0.375</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="10" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>8</v>
+      <c r="D7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="0"/>
+      <c r="G7" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,11 +503,12 @@
       <c r="C8" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="D8" s="11" t="s">
         <v>15</v>
+      </c>
+      <c r="F8" s="0"/>
+      <c r="G8" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -502,7 +530,7 @@
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -540,167 +568,167 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC1" s="0"/>
       <c r="AD1" s="0"/>
       <c r="AE1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="10" t="n">
+      <c r="A2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="n">
+      <c r="C2" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>40</v>
+      <c r="D2" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="9" t="n">
+        <v>41</v>
+      </c>
+      <c r="I2" s="10" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="J2" s="10" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="K2" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="J2" s="9" t="n">
+      <c r="L2" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="K2" s="9" t="n">
+      <c r="M2" s="10" t="n">
+        <v>0.354166666666667</v>
+      </c>
+      <c r="N2" s="10" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="O2" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="L2" s="9" t="n">
+      <c r="P2" s="10" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="S2" s="10" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="T2" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="M2" s="9" t="n">
+      <c r="U2" s="10" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="V2" s="10" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="W2" s="10" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="N2" s="9" t="n">
+      <c r="X2" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="O2" s="9" t="n">
+      <c r="Y2" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="P2" s="9" t="n">
+      <c r="Z2" s="10" t="n">
         <v>0.6875</v>
       </c>
-      <c r="S2" s="9" t="n">
+      <c r="AA2" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="T2" s="9" t="n">
-        <v>0.708333333333333</v>
-      </c>
-      <c r="U2" s="9" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="V2" s="9" t="n">
-        <v>0.708333333333333</v>
-      </c>
-      <c r="W2" s="9" t="n">
-        <v>0.354166666666667</v>
-      </c>
-      <c r="X2" s="9" t="n">
-        <v>0.708333333333333</v>
-      </c>
-      <c r="Y2" s="9" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="Z2" s="9" t="n">
-        <v>0.6875</v>
-      </c>
-      <c r="AA2" s="9" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="AB2" s="9" t="n">
+      <c r="AB2" s="10" t="n">
         <v>0.6875</v>
       </c>
       <c r="AC2" s="0"/>
@@ -708,49 +736,49 @@
       <c r="AE2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="10" t="n">
+      <c r="A3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
       <c r="G3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="9" t="n">
+        <v>43</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="10" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="P3" s="9" t="n">
+      <c r="P3" s="10" t="n">
         <v>0.833333333333333</v>
       </c>
-      <c r="Q3" s="9" t="n">
+      <c r="Q3" s="10" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="R3" s="9" t="n">
+      <c r="R3" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="9" t="n">
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="10" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="X3" s="9" t="n">
+      <c r="X3" s="10" t="n">
         <v>0.833333333333333</v>
       </c>
-      <c r="Y3" s="9" t="n">
+      <c r="Y3" s="10" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="Z3" s="9" t="n">
+      <c r="Z3" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
       <c r="AC3" s="0"/>
@@ -789,36 +817,36 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="7" t="s">
         <v>45</v>
       </c>
+      <c r="E1" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="8" t="n">
+      <c r="A2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="9" t="n">
         <v>42773</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="D2" s="10" t="n">
         <v>0.375</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -839,7 +867,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -853,34 +881,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="8" t="n">
+      <c r="A2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="9" t="n">
         <v>42773</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="8" t="n">
+        <v>42</v>
+      </c>
+      <c r="B3" s="9" t="n">
         <v>42776</v>
       </c>
       <c r="C3" s="1" t="n">

</xml_diff>

<commit_message>
can now override RO using RO column
</commit_message>
<xml_diff>
--- a/data/shifty.xlsx
+++ b/data/shifty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Shifts" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">Beast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RO</t>
   </si>
   <si>
     <t xml:space="preserve">Mon start P</t>
@@ -361,7 +364,7 @@
   </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -527,9 +530,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -542,28 +545,29 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="2" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="9.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="2" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="9.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="3" width="5.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="3" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="3" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="32" style="3" width="14.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="2" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="2" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="2" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="3" width="5.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="3" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="3" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="33" style="3" width="14.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,7 +595,7 @@
       <c r="H1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -651,9 +655,12 @@
       <c r="AB1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AC1" s="0"/>
+      <c r="AC1" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="AD1" s="0"/>
       <c r="AE1" s="0"/>
+      <c r="AF1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
@@ -666,78 +673,78 @@
         <v>0</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="10" t="n">
+        <v>42</v>
+      </c>
+      <c r="J2" s="10" t="n">
         <v>0.375</v>
       </c>
-      <c r="J2" s="10" t="n">
+      <c r="K2" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="K2" s="10" t="n">
+      <c r="L2" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="L2" s="10" t="n">
+      <c r="M2" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="M2" s="10" t="n">
+      <c r="N2" s="10" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="N2" s="10" t="n">
+      <c r="O2" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="O2" s="10" t="n">
+      <c r="P2" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="P2" s="10" t="n">
+      <c r="Q2" s="10" t="n">
         <v>0.6875</v>
       </c>
-      <c r="S2" s="10" t="n">
+      <c r="T2" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="T2" s="10" t="n">
+      <c r="U2" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="U2" s="10" t="n">
+      <c r="V2" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="V2" s="10" t="n">
+      <c r="W2" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="W2" s="10" t="n">
+      <c r="X2" s="10" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="X2" s="10" t="n">
+      <c r="Y2" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="Y2" s="10" t="n">
+      <c r="Z2" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="Z2" s="10" t="n">
+      <c r="AA2" s="10" t="n">
         <v>0.6875</v>
       </c>
-      <c r="AA2" s="10" t="n">
+      <c r="AB2" s="10" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="AB2" s="10" t="n">
+      <c r="AC2" s="10" t="n">
         <v>0.6875</v>
       </c>
-      <c r="AC2" s="0"/>
       <c r="AD2" s="0"/>
       <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3" s="11" t="n">
         <v>6</v>
@@ -745,45 +752,48 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="G3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="12"/>
+        <v>44</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
-      <c r="O3" s="10" t="n">
+      <c r="O3" s="12"/>
+      <c r="P3" s="10" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="P3" s="10" t="n">
+      <c r="Q3" s="10" t="n">
         <v>0.833333333333333</v>
       </c>
-      <c r="Q3" s="10" t="n">
+      <c r="R3" s="10" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="R3" s="10" t="n">
+      <c r="S3" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="S3" s="12"/>
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
       <c r="V3" s="12"/>
-      <c r="W3" s="10" t="n">
+      <c r="W3" s="12"/>
+      <c r="X3" s="10" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="X3" s="10" t="n">
+      <c r="Y3" s="10" t="n">
         <v>0.833333333333333</v>
       </c>
-      <c r="Y3" s="10" t="n">
+      <c r="Z3" s="10" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="Z3" s="10" t="n">
+      <c r="AA3" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="AC3" s="0"/>
       <c r="AD3" s="0"/>
       <c r="AE3" s="0"/>
+      <c r="AF3" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -823,13 +833,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,7 +856,7 @@
         <v>0.375</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -884,13 +894,13 @@
         <v>17</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -901,12 +911,12 @@
         <v>42773</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3" s="9" t="n">
         <v>42776</v>

</xml_diff>